<commit_message>
Correção no nome da planilha
</commit_message>
<xml_diff>
--- a/Regioes.xlsx
+++ b/Regioes.xlsx
@@ -3,12 +3,12 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_8A951CE47955B3A2760729FE361B1FD31C1F5E6E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F045FFEC-83FD-4B8E-85AA-C5225695B54E}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_8A951CE47955B3A2760729FE361B1FD31C1F5E6E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5ECB49AE-20AC-4259-9042-7DCDACB3AB46}"/>
   <bookViews>
     <workbookView xWindow="-25320" yWindow="-3165" windowWidth="25440" windowHeight="15270" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Regioes" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519"/>
 </workbook>
@@ -100,6 +100,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>